<commit_message>
Finalización del ejercicio 13
</commit_message>
<xml_diff>
--- a/Syllabus - ClearMinds.xlsx
+++ b/Syllabus - ClearMinds.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\6. Empresa\RETOS TÉCNICOS\Clear Minds\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5EEACDAD-02B6-4950-B82C-9E2272F9916F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5148B5D-91CB-4BE2-8C2C-DA663A3C850A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{24A60BB0-8A34-4F46-A842-3DB1738592D3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{24A60BB0-8A34-4F46-A842-3DB1738592D3}"/>
   </bookViews>
   <sheets>
     <sheet name="ClearMinds" sheetId="1" r:id="rId1"/>
@@ -27,18 +27,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
-    <t>EVALUACIÓN JAVA STANDARD</t>
-  </si>
-  <si>
-    <t>16 Ejemplo Evaluación Java Standard Edition - LISTAS</t>
-  </si>
-  <si>
-    <t>14 Repaso Evaluación 2</t>
-  </si>
-  <si>
-    <t>13 Repaso Evaluación Java Standard Edition</t>
-  </si>
-  <si>
     <t>Evaluación</t>
   </si>
   <si>
@@ -49,6 +37,18 @@
   </si>
   <si>
     <t>Directorio</t>
+  </si>
+  <si>
+    <t>13 Repaso Evaluación Java Standard Edition (EvaluacionBUG)</t>
+  </si>
+  <si>
+    <t>14 Repaso Evaluación 2 (JSEBEvaluación)</t>
+  </si>
+  <si>
+    <t>16 Ejemplo Evaluación Java Standard Edition - LISTAS (Evaluacion1BryanUmanaGomez)</t>
+  </si>
+  <si>
+    <t>EVALUACIÓN JAVA STANDARD JavaBryanUmanaGomez)</t>
   </si>
 </sst>
 </file>
@@ -64,7 +64,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -86,6 +86,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -117,16 +123,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -444,77 +451,77 @@
   <dimension ref="B2:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="48" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="78.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="3">
+      <c r="B2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B3" s="4"/>
-      <c r="C3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="3">
+      <c r="B3" s="3"/>
+      <c r="C3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="2">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B4" s="4"/>
-      <c r="C4" s="3" t="s">
+      <c r="B4" s="3"/>
+      <c r="C4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B5" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="5">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="4"/>
+      <c r="C6" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="D4" s="3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" s="1">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="2"/>
-      <c r="C6" s="1" t="s">
-        <v>2</v>
       </c>
       <c r="D6" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="2"/>
+      <c r="B7" s="4"/>
       <c r="C7" s="1" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D7" s="1">
         <v>13</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B8" s="2"/>
+      <c r="B8" s="4"/>
       <c r="C8" s="1" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D8" s="1">
         <v>13</v>

</xml_diff>